<commit_message>
error handle pt 1 + fix demo
</commit_message>
<xml_diff>
--- a/Arrivati.xlsx
+++ b/Arrivati.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,20 +436,10 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>nome</t>
+          <t>cognome</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>cognome</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>nome completo</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Arrivo</t>
         </is>
@@ -461,22 +451,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>francesco</t>
+          <t>totti</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>totti</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>francesco_totti</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>No</t>
+          <t>Arrivato</t>
         </is>
       </c>
     </row>
@@ -486,22 +466,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>donald</t>
+          <t>trump</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>trump</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>donald_trump</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Arrivato</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -511,20 +481,10 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>manuela</t>
+          <t>arcuri</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
-        <is>
-          <t>arcuri</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>manuela_arcuri</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -536,20 +496,10 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>elsa</t>
+          <t>frozen</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
-        <is>
-          <t>frozen</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>elsa_frozen</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -561,20 +511,10 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>giorgia</t>
+          <t>meloni</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
-        <is>
-          <t>meloni</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>giorgia_meloni</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -586,20 +526,10 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>napoleone</t>
+          <t>bonaparte</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
-        <is>
-          <t>bonaparte</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>napoleone_bonaparte</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -611,22 +541,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>gruppo</t>
+          <t>pooh</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>pooh</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>gruppo_pooh</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Arrivato</t>
+          <t>No</t>
         </is>
       </c>
     </row>

</xml_diff>